<commit_message>
Added files and created OrderHistory branch
</commit_message>
<xml_diff>
--- a/NMMakerFnFEvent_BOM.xlsx
+++ b/NMMakerFnFEvent_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13728" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13725" windowHeight="7380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AR List" sheetId="1" r:id="rId1"/>
@@ -1299,7 +1299,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>893445</xdr:colOff>
+      <xdr:colOff>883920</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>893445</xdr:rowOff>
     </xdr:to>
@@ -2317,7 +2317,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>910329</xdr:colOff>
+      <xdr:colOff>881754</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>861060</xdr:rowOff>
     </xdr:to>
@@ -2600,7 +2600,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>893115</xdr:colOff>
+      <xdr:colOff>883590</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>861061</xdr:rowOff>
     </xdr:to>
@@ -2902,16 +2902,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>26</v>
       </c>
@@ -2937,7 +2937,7 @@
       <c r="D2" s="70"/>
       <c r="E2" s="71"/>
     </row>
-    <row r="3" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -2965,7 +2965,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="79"/>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -2976,7 +2976,7 @@
       <c r="D5" s="9"/>
       <c r="E5" s="80"/>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
         <v>27</v>
       </c>
@@ -2985,7 +2985,7 @@
       <c r="D6" s="70"/>
       <c r="E6" s="71"/>
     </row>
-    <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
@@ -3020,7 +3020,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
         <v>28</v>
       </c>
@@ -3029,7 +3029,7 @@
       <c r="D10" s="70"/>
       <c r="E10" s="71"/>
     </row>
-    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
@@ -3053,7 +3053,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -3062,7 +3062,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
@@ -3071,7 +3071,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="69" t="s">
         <v>30</v>
       </c>
@@ -3080,7 +3080,7 @@
       <c r="D15" s="70"/>
       <c r="E15" s="71"/>
     </row>
-    <row r="16" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
@@ -3106,7 +3106,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>35</v>
       </c>
@@ -3115,7 +3115,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
         <v>61</v>
       </c>
@@ -3124,7 +3124,7 @@
       <c r="D19" s="70"/>
       <c r="E19" s="71"/>
     </row>
-    <row r="20" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>7</v>
       </c>
@@ -3137,7 +3137,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
@@ -3146,7 +3146,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -3168,7 +3168,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>31</v>
       </c>
@@ -3177,7 +3177,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
@@ -3190,7 +3190,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -3203,7 +3203,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>36</v>
       </c>
@@ -3216,7 +3216,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>36</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="81" t="s">
         <v>33</v>
       </c>
@@ -3240,7 +3240,7 @@
       <c r="D28" s="81"/>
       <c r="E28" s="81"/>
     </row>
-    <row r="29" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>37</v>
       </c>
@@ -3253,7 +3253,7 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>37</v>
       </c>
@@ -3266,7 +3266,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>37</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>37</v>
       </c>
@@ -3294,7 +3294,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>66</v>
       </c>
@@ -3307,7 +3307,7 @@
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
     </row>
-    <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>37</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>69</v>
       </c>
@@ -3333,7 +3333,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="82" t="s">
         <v>40</v>
       </c>
@@ -3342,7 +3342,7 @@
       <c r="D36" s="83"/>
       <c r="E36" s="83"/>
     </row>
-    <row r="37" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>41</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>41</v>
       </c>
@@ -3366,7 +3366,7 @@
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>44</v>
       </c>
@@ -3377,7 +3377,7 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>45</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>11</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>46</v>
       </c>
@@ -3418,7 +3418,7 @@
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>48</v>
       </c>
@@ -3429,7 +3429,7 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>50</v>
       </c>
@@ -3440,7 +3440,7 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>52</v>
       </c>
@@ -3451,7 +3451,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="72" t="s">
         <v>75</v>
       </c>
@@ -3460,7 +3460,7 @@
       <c r="D46" s="73"/>
       <c r="E46" s="74"/>
     </row>
-    <row r="47" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>76</v>
       </c>
@@ -3473,7 +3473,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>78</v>
       </c>
@@ -3516,23 +3516,24 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="71.45" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="83.109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="56" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="134.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="84" t="s">
         <v>99</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="46" t="s">
         <v>86</v>
       </c>
@@ -3604,7 +3605,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="46" t="s">
         <v>121</v>
       </c>
@@ -3634,7 +3635,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">
         <v>88</v>
       </c>
@@ -3657,7 +3658,7 @@
         <v>644.65000000000032</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="46" t="s">
         <v>90</v>
       </c>
@@ -3678,7 +3679,7 @@
         <v>72.680000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="52" t="s">
         <v>91</v>
       </c>
@@ -3702,7 +3703,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="46" t="s">
         <v>93</v>
       </c>
@@ -3718,7 +3719,7 @@
       </c>
       <c r="F7" s="57"/>
     </row>
-    <row r="8" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="46" t="s">
         <v>95</v>
       </c>
@@ -3734,7 +3735,7 @@
       </c>
       <c r="F8" s="57"/>
     </row>
-    <row r="9" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>8</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>217.56</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>10</v>
       </c>
@@ -3773,7 +3774,7 @@
       <c r="F10" s="57"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>171</v>
       </c>
@@ -3792,7 +3793,7 @@
       <c r="F11" s="57"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="12" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="48" t="s">
         <v>171</v>
       </c>
@@ -3811,7 +3812,7 @@
       <c r="F12" s="57"/>
       <c r="K12" s="39"/>
     </row>
-    <row r="13" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="48" t="s">
         <v>187</v>
       </c>
@@ -3829,7 +3830,7 @@
       </c>
       <c r="F13" s="57"/>
     </row>
-    <row r="14" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C14" s="22" t="s">
         <v>96</v>
       </c>
@@ -3843,7 +3844,7 @@
       </c>
       <c r="F14" s="57"/>
     </row>
-    <row r="15" spans="1:16" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="84" t="s">
         <v>98</v>
       </c>
@@ -3857,7 +3858,7 @@
       </c>
       <c r="F15" s="57"/>
     </row>
-    <row r="16" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="46" t="s">
         <v>118</v>
       </c>
@@ -3878,7 +3879,7 @@
         <v>54.28</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
         <v>179</v>
       </c>
@@ -3899,7 +3900,7 @@
         <v>14.31</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="50" t="s">
         <v>125</v>
       </c>
@@ -3924,7 +3925,7 @@
       <c r="I18" s="29"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="50" t="s">
         <v>126</v>
       </c>
@@ -3949,7 +3950,7 @@
       <c r="I19" s="29"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="50" t="s">
         <v>124</v>
       </c>
@@ -3973,7 +3974,7 @@
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="50" t="s">
         <v>127</v>
       </c>
@@ -3996,7 +3997,7 @@
       </c>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="50" t="s">
         <v>128</v>
       </c>
@@ -4014,7 +4015,7 @@
       <c r="F22" s="57"/>
       <c r="G22" s="39"/>
     </row>
-    <row r="23" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C23" s="22" t="s">
         <v>96</v>
       </c>
@@ -4028,7 +4029,7 @@
       </c>
       <c r="F23" s="57"/>
     </row>
-    <row r="24" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="84" t="s">
         <v>97</v>
       </c>
@@ -4042,7 +4043,7 @@
       </c>
       <c r="F24" s="57"/>
     </row>
-    <row r="25" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="46" t="s">
         <v>120</v>
       </c>
@@ -4063,7 +4064,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>181</v>
       </c>
@@ -4080,7 +4081,7 @@
       <c r="F26" s="57"/>
       <c r="G26" s="39"/>
     </row>
-    <row r="27" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="48" t="s">
         <v>171</v>
       </c>
@@ -4105,7 +4106,7 @@
       </c>
       <c r="H27" s="51"/>
     </row>
-    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C28" s="22" t="s">
         <v>96</v>
       </c>
@@ -4119,7 +4120,7 @@
       </c>
       <c r="F28" s="57"/>
     </row>
-    <row r="29" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="84" t="s">
         <v>147</v>
       </c>
@@ -4133,7 +4134,7 @@
       </c>
       <c r="F29" s="57"/>
     </row>
-    <row r="30" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="47" t="s">
         <v>152</v>
       </c>
@@ -4154,7 +4155,7 @@
       </c>
       <c r="G30" s="39"/>
     </row>
-    <row r="31" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="47" t="s">
         <v>153</v>
       </c>
@@ -4174,7 +4175,7 @@
       </c>
       <c r="G31" s="39"/>
     </row>
-    <row r="32" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="47" t="s">
         <v>154</v>
       </c>
@@ -4194,7 +4195,7 @@
       </c>
       <c r="G32" s="39"/>
     </row>
-    <row r="33" spans="1:7" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="47" t="s">
         <v>155</v>
       </c>
@@ -4214,7 +4215,7 @@
       </c>
       <c r="G33" s="39"/>
     </row>
-    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C34" s="22" t="s">
         <v>96</v>
       </c>
@@ -4231,7 +4232,7 @@
         <v>10.335000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="64"/>
       <c r="B35" s="18"/>
       <c r="C35" s="63"/>
@@ -4244,7 +4245,7 @@
       <c r="F35" s="60"/>
       <c r="G35" s="39"/>
     </row>
-    <row r="36" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="65"/>
       <c r="B36" s="66"/>
       <c r="C36" s="24" t="s">
@@ -4260,10 +4261,10 @@
       </c>
       <c r="F36" s="57"/>
     </row>
-    <row r="37" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F37" s="57"/>
     </row>
-    <row r="38" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C38" s="24" t="s">
         <v>198</v>
       </c>
@@ -4306,13 +4307,17 @@
     <hyperlink ref="A13" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="87" orientation="landscape" r:id="rId23"/>
+  <pageSetup scale="57" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId23"/>
   <headerFooter>
     <oddHeader>&amp;LIntel Maker Nation Presents&amp;CA Friends and Family Event&amp;RApril 2016</oddHeader>
   </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="25" max="3" man="1"/>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="14" max="16383" man="1"/>
+    <brk id="23" max="16383" man="1"/>
   </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="7" max="1048575" man="1"/>
+  </colBreaks>
   <drawing r:id="rId24"/>
 </worksheet>
 </file>
@@ -4325,19 +4330,19 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>100</v>
       </c>
@@ -4363,7 +4368,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -4383,7 +4388,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4406,7 +4411,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -4432,7 +4437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -4442,11 +4447,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="37"/>
       <c r="E6" s="37"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -4456,7 +4461,7 @@
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -4466,18 +4471,18 @@
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
     </row>
-    <row r="11" spans="1:9" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="35" t="s">
         <v>131</v>
       </c>
@@ -4503,7 +4508,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -4518,7 +4523,7 @@
       <c r="H12" s="35"/>
       <c r="I12" s="35"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>144</v>
       </c>
@@ -4526,7 +4531,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -4543,7 +4548,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>135</v>
       </c>
@@ -4557,7 +4562,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>136</v>
       </c>
@@ -4571,7 +4576,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -4588,7 +4593,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>135</v>
       </c>
@@ -4602,7 +4607,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>136</v>
       </c>
@@ -4616,7 +4621,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>138</v>
       </c>
@@ -4633,7 +4638,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>136</v>
       </c>
@@ -4647,7 +4652,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>135</v>
       </c>
@@ -4661,7 +4666,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>136</v>
       </c>
@@ -4669,7 +4674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
updated files from David and Kids build
</commit_message>
<xml_diff>
--- a/NMMakerFnFEvent_BOM.xlsx
+++ b/NMMakerFnFEvent_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13725" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13728" windowHeight="7380" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AR List" sheetId="1" r:id="rId1"/>
@@ -820,7 +820,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -998,15 +998,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="dotted">
-        <color auto="1"/>
-      </diagonal>
-    </border>
     <border>
       <left/>
       <right style="medium">
@@ -1100,10 +1091,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1167,7 +1154,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1221,6 +1208,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2902,16 +2893,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -2928,115 +2919,115 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-    </row>
-    <row r="3" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="69"/>
+    </row>
+    <row r="3" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="73" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="76" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="76"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="79"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="77"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="77"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="80"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="69" t="s">
+      <c r="E5" s="78"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="71"/>
-    </row>
-    <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="69"/>
+    </row>
+    <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="73" t="s">
         <v>55</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="76"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="77"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="69" t="s">
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="71"/>
-    </row>
-    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="69"/>
+    </row>
+    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="76" t="s">
         <v>82</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -3044,43 +3035,43 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="79"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="79"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="80"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="69" t="s">
+    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
-    </row>
-    <row r="16" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
+    </row>
+    <row r="16" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
@@ -3097,7 +3088,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
@@ -3106,7 +3097,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>35</v>
       </c>
@@ -3115,16 +3106,16 @@
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="69" t="s">
+    <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="71"/>
-    </row>
-    <row r="20" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="69"/>
+    </row>
+    <row r="20" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>7</v>
       </c>
@@ -3137,7 +3128,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
@@ -3146,7 +3137,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -3168,7 +3159,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>31</v>
       </c>
@@ -3177,7 +3168,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
@@ -3190,7 +3181,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -3203,7 +3194,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>36</v>
       </c>
@@ -3216,7 +3207,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>36</v>
       </c>
@@ -3231,16 +3222,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="81" t="s">
+    <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-    </row>
-    <row r="29" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+    </row>
+    <row r="29" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>37</v>
       </c>
@@ -3253,7 +3244,7 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>37</v>
       </c>
@@ -3266,7 +3257,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>37</v>
       </c>
@@ -3281,7 +3272,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>37</v>
       </c>
@@ -3294,7 +3285,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>66</v>
       </c>
@@ -3307,7 +3298,7 @@
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
     </row>
-    <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>37</v>
       </c>
@@ -3320,7 +3311,7 @@
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>69</v>
       </c>
@@ -3333,62 +3324,62 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="82" t="s">
+    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="83"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-    </row>
-    <row r="37" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="81"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
+    </row>
+    <row r="37" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="78" t="s">
+      <c r="C37" s="76" t="s">
         <v>74</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="79"/>
+      <c r="C38" s="77"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="79"/>
+      <c r="C39" s="77"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="80"/>
+      <c r="C40" s="78"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>11</v>
       </c>
@@ -3405,62 +3396,62 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="76" t="s">
         <v>74</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="79"/>
+      <c r="C43" s="77"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="79"/>
+      <c r="C44" s="77"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="80"/>
+      <c r="C45" s="78"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="72" t="s">
+    <row r="46" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="74"/>
-    </row>
-    <row r="47" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="71"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="72"/>
+    </row>
+    <row r="47" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>76</v>
       </c>
@@ -3473,7 +3464,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>78</v>
       </c>
@@ -3515,60 +3506,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="71.45" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="134.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="56" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="134.44140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="40" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="53" t="s">
         <v>193</v>
       </c>
       <c r="H1" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="N1" s="42" t="s">
         <v>171</v>
       </c>
       <c r="O1" s="35" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="44" t="s">
         <v>86</v>
       </c>
       <c r="B2" s="19"/>
@@ -3581,7 +3572,7 @@
       <c r="E2" s="25">
         <v>399.2</v>
       </c>
-      <c r="F2" s="57"/>
+      <c r="F2" s="55"/>
       <c r="H2" t="s">
         <v>166</v>
       </c>
@@ -3605,8 +3596,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+    <row r="3" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="44" t="s">
         <v>121</v>
       </c>
       <c r="B3" s="19"/>
@@ -3620,7 +3611,7 @@
       <c r="E3" s="25">
         <v>48</v>
       </c>
-      <c r="F3" s="57"/>
+      <c r="F3" s="55"/>
       <c r="J3" s="35" t="s">
         <v>192</v>
       </c>
@@ -3635,8 +3626,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="44" t="s">
         <v>88</v>
       </c>
       <c r="B4" s="19"/>
@@ -3649,7 +3640,7 @@
       <c r="E4" s="25">
         <v>47.2</v>
       </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="55"/>
       <c r="J4" t="s">
         <v>197</v>
       </c>
@@ -3658,8 +3649,8 @@
         <v>644.65000000000032</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+    <row r="5" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="44" t="s">
         <v>90</v>
       </c>
       <c r="B5" s="19"/>
@@ -3672,39 +3663,39 @@
       <c r="E5" s="25">
         <v>63.2</v>
       </c>
-      <c r="F5" s="57">
+      <c r="F5" s="55">
         <v>3</v>
       </c>
       <c r="G5" s="25">
         <v>72.680000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+    <row r="6" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="60">
         <v>10.36</v>
       </c>
-      <c r="E6" s="61">
+      <c r="E6" s="59">
         <v>196.84</v>
       </c>
-      <c r="F6" s="58">
+      <c r="F6" s="56">
         <v>3</v>
       </c>
-      <c r="G6" s="61">
+      <c r="G6" s="59">
         <v>227.92</v>
       </c>
       <c r="H6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="46" t="s">
+    <row r="7" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="44" t="s">
         <v>93</v>
       </c>
       <c r="B7" s="19"/>
@@ -3717,10 +3708,10 @@
       <c r="E7" s="25">
         <v>7.2</v>
       </c>
-      <c r="F7" s="57"/>
-    </row>
-    <row r="8" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="46" t="s">
+      <c r="F7" s="55"/>
+    </row>
+    <row r="8" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="44" t="s">
         <v>95</v>
       </c>
       <c r="B8" s="19"/>
@@ -3733,10 +3724,10 @@
       <c r="E8" s="25">
         <v>20</v>
       </c>
-      <c r="F8" s="57"/>
-    </row>
-    <row r="9" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
+      <c r="F8" s="55"/>
+    </row>
+    <row r="9" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="20"/>
@@ -3749,15 +3740,15 @@
       <c r="E9" s="25">
         <v>207.2</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="55">
         <v>1</v>
       </c>
       <c r="G9" s="25">
         <v>217.56</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
+    <row r="10" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="45" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="20"/>
@@ -3771,11 +3762,11 @@
         <f>26*20</f>
         <v>520</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="K10" s="39"/>
-    </row>
-    <row r="11" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="48" t="s">
+      <c r="F10" s="55"/>
+      <c r="K10" s="37"/>
+    </row>
+    <row r="11" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
         <v>171</v>
       </c>
       <c r="B11" s="17"/>
@@ -3790,11 +3781,11 @@
         <f>7.89*4</f>
         <v>31.56</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="K11" s="39"/>
-    </row>
-    <row r="12" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
+      <c r="F11" s="55"/>
+      <c r="K11" s="37"/>
+    </row>
+    <row r="12" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="46" t="s">
         <v>171</v>
       </c>
       <c r="B12" s="17"/>
@@ -3809,11 +3800,11 @@
         <f>7.99</f>
         <v>7.99</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="K12" s="39"/>
-    </row>
-    <row r="13" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+      <c r="F12" s="55"/>
+      <c r="K12" s="37"/>
+    </row>
+    <row r="13" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="46" t="s">
         <v>187</v>
       </c>
       <c r="B13" s="17"/>
@@ -3828,9 +3819,9 @@
         <f>8.99*7</f>
         <v>62.93</v>
       </c>
-      <c r="F13" s="57"/>
-    </row>
-    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F13" s="55"/>
+    </row>
+    <row r="14" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="C14" s="22" t="s">
         <v>96</v>
       </c>
@@ -3842,24 +3833,24 @@
         <f>SUM(E2:E13)</f>
         <v>1611.3200000000002</v>
       </c>
-      <c r="F14" s="57"/>
-    </row>
-    <row r="15" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="84" t="s">
+      <c r="F14" s="55"/>
+    </row>
+    <row r="15" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="40" t="s">
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="F15" s="57"/>
-    </row>
-    <row r="16" spans="1:16" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="46" t="s">
+      <c r="F15" s="55"/>
+    </row>
+    <row r="16" spans="1:16" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="44" t="s">
         <v>118</v>
       </c>
       <c r="B16" s="19"/>
@@ -3872,15 +3863,15 @@
       <c r="E16" s="25">
         <v>47.2</v>
       </c>
-      <c r="F16" s="57">
+      <c r="F16" s="55">
         <v>3</v>
       </c>
       <c r="G16" s="25">
         <v>54.28</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50" t="s">
+    <row r="17" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="48" t="s">
         <v>179</v>
       </c>
       <c r="B17" s="33"/>
@@ -3893,19 +3884,19 @@
       <c r="E17" s="25">
         <v>12.44</v>
       </c>
-      <c r="F17" s="59">
+      <c r="F17" s="57">
         <v>3</v>
       </c>
       <c r="G17" s="25">
         <v>14.31</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
+    <row r="18" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="48" t="s">
         <v>125</v>
       </c>
       <c r="B18" s="32"/>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="39" t="s">
         <v>158</v>
       </c>
       <c r="D18" s="25">
@@ -3915,7 +3906,7 @@
       <c r="E18" s="25">
         <v>7.32</v>
       </c>
-      <c r="F18" s="59">
+      <c r="F18" s="57">
         <v>6</v>
       </c>
       <c r="G18" s="25">
@@ -3925,8 +3916,8 @@
       <c r="I18" s="29"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50" t="s">
+    <row r="19" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="48" t="s">
         <v>126</v>
       </c>
       <c r="B19" s="33"/>
@@ -3940,7 +3931,7 @@
       <c r="E19" s="25">
         <v>19.62</v>
       </c>
-      <c r="F19" s="59">
+      <c r="F19" s="57">
         <v>9</v>
       </c>
       <c r="G19" s="25">
@@ -3950,8 +3941,8 @@
       <c r="I19" s="29"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+    <row r="20" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="48" t="s">
         <v>124</v>
       </c>
       <c r="B20" s="32"/>
@@ -3965,7 +3956,7 @@
       <c r="E20" s="25">
         <v>5.2</v>
       </c>
-      <c r="F20" s="59">
+      <c r="F20" s="57">
         <v>6</v>
       </c>
       <c r="G20" s="25">
@@ -3974,8 +3965,8 @@
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50" t="s">
+    <row r="21" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="48" t="s">
         <v>127</v>
       </c>
       <c r="B21" s="33"/>
@@ -3989,7 +3980,7 @@
       <c r="E21" s="25">
         <v>8.2200000000000006</v>
       </c>
-      <c r="F21" s="59">
+      <c r="F21" s="57">
         <v>9</v>
       </c>
       <c r="G21" s="25">
@@ -3997,8 +3988,8 @@
       </c>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="50" t="s">
+    <row r="22" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="48" t="s">
         <v>128</v>
       </c>
       <c r="B22" s="20"/>
@@ -4012,10 +4003,10 @@
       <c r="E22" s="25">
         <v>43.2</v>
       </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="39"/>
-    </row>
-    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F22" s="55"/>
+      <c r="G22" s="37"/>
+    </row>
+    <row r="23" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="C23" s="22" t="s">
         <v>96</v>
       </c>
@@ -4027,24 +4018,24 @@
         <f>SUM(E16:E22)</f>
         <v>143.20000000000002</v>
       </c>
-      <c r="F23" s="57"/>
-    </row>
-    <row r="24" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="84" t="s">
+      <c r="F23" s="55"/>
+    </row>
+    <row r="24" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="84"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="40" t="s">
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="F24" s="57"/>
-    </row>
-    <row r="25" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="46" t="s">
+      <c r="F24" s="55"/>
+    </row>
+    <row r="25" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="44" t="s">
         <v>120</v>
       </c>
       <c r="B25" s="20"/>
@@ -4057,15 +4048,15 @@
       <c r="E25" s="25">
         <v>24</v>
       </c>
-      <c r="F25" s="57">
+      <c r="F25" s="55">
         <v>3</v>
       </c>
       <c r="G25" s="25">
         <v>27.6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50" t="s">
+    <row r="26" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="48" t="s">
         <v>181</v>
       </c>
       <c r="B26" s="20"/>
@@ -4078,11 +4069,11 @@
       <c r="E26" s="25">
         <v>124.4</v>
       </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="39"/>
-    </row>
-    <row r="27" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="48" t="s">
+      <c r="F26" s="55"/>
+      <c r="G26" s="37"/>
+    </row>
+    <row r="27" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="46" t="s">
         <v>171</v>
       </c>
       <c r="B27" s="20"/>
@@ -4097,16 +4088,16 @@
         <f>20.99*2</f>
         <v>41.98</v>
       </c>
-      <c r="F27" s="57">
+      <c r="F27" s="55">
         <v>5</v>
       </c>
       <c r="G27" s="25">
         <f>E27+11.48</f>
         <v>53.459999999999994</v>
       </c>
-      <c r="H27" s="51"/>
-    </row>
-    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H27" s="49"/>
+    </row>
+    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="C28" s="22" t="s">
         <v>96</v>
       </c>
@@ -4118,24 +4109,24 @@
         <f>SUM(E25:E27)</f>
         <v>190.38</v>
       </c>
-      <c r="F28" s="57"/>
-    </row>
-    <row r="29" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="84" t="s">
+      <c r="F28" s="55"/>
+    </row>
+    <row r="29" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="40" t="s">
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="57"/>
-    </row>
-    <row r="30" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="47" t="s">
+      <c r="F29" s="55"/>
+    </row>
+    <row r="30" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="45" t="s">
         <v>152</v>
       </c>
       <c r="B30" s="17"/>
@@ -4150,13 +4141,13 @@
         <f>D30*20</f>
         <v>52</v>
       </c>
-      <c r="F30" s="60">
+      <c r="F30" s="58">
         <v>1.82</v>
       </c>
-      <c r="G30" s="39"/>
-    </row>
-    <row r="31" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="47" t="s">
+      <c r="G30" s="37"/>
+    </row>
+    <row r="31" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="45" t="s">
         <v>153</v>
       </c>
       <c r="B31" s="17"/>
@@ -4170,13 +4161,13 @@
         <f t="shared" ref="E31:E33" si="0">D31*20</f>
         <v>31</v>
       </c>
-      <c r="F31" s="60">
+      <c r="F31" s="58">
         <v>4.55</v>
       </c>
-      <c r="G31" s="39"/>
-    </row>
-    <row r="32" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="47" t="s">
+      <c r="G31" s="37"/>
+    </row>
+    <row r="32" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="45" t="s">
         <v>154</v>
       </c>
       <c r="B32" s="17"/>
@@ -4190,13 +4181,13 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="F32" s="60">
+      <c r="F32" s="58">
         <v>1.885</v>
       </c>
-      <c r="G32" s="39"/>
-    </row>
-    <row r="33" spans="1:7" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="47" t="s">
+      <c r="G32" s="37"/>
+    </row>
+    <row r="33" spans="1:7" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="45" t="s">
         <v>155</v>
       </c>
       <c r="B33" s="17"/>
@@ -4210,12 +4201,12 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="F33" s="60">
+      <c r="F33" s="58">
         <v>2.08</v>
       </c>
-      <c r="G33" s="39"/>
-    </row>
-    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G33" s="37"/>
+    </row>
+    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C34" s="22" t="s">
         <v>96</v>
       </c>
@@ -4227,27 +4218,27 @@
         <f>SUM(E30:E33)</f>
         <v>172</v>
       </c>
-      <c r="F34" s="60">
+      <c r="F34" s="58">
         <f>SUM(F30:F33)</f>
         <v>10.335000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="64"/>
+    <row r="35" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="62"/>
       <c r="B35" s="18"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="67" t="s">
+      <c r="C35" s="61"/>
+      <c r="D35" s="65" t="s">
         <v>183</v>
       </c>
-      <c r="E35" s="68" t="s">
+      <c r="E35" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="60"/>
-      <c r="G35" s="39"/>
-    </row>
-    <row r="36" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="65"/>
-      <c r="B36" s="66"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="37"/>
+    </row>
+    <row r="36" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="63"/>
+      <c r="B36" s="64"/>
       <c r="C36" s="24" t="s">
         <v>200</v>
       </c>
@@ -4259,12 +4250,12 @@
         <f>SUM(E14,E23,E28,E34)/20</f>
         <v>105.845</v>
       </c>
-      <c r="F36" s="57"/>
-    </row>
-    <row r="37" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F37" s="57"/>
-    </row>
-    <row r="38" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F36" s="55"/>
+    </row>
+    <row r="37" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F37" s="55"/>
+    </row>
+    <row r="38" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="24" t="s">
         <v>198</v>
       </c>
@@ -4272,8 +4263,8 @@
         <f>O4</f>
         <v>644.65000000000032</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="57"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4326,33 +4317,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>100</v>
       </c>
       <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="83" t="s">
         <v>103</v>
       </c>
       <c r="F1" t="s">
@@ -4368,14 +4359,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="83" t="s">
         <v>112</v>
       </c>
       <c r="G2" t="s">
@@ -4388,14 +4379,14 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="83" t="s">
         <v>112</v>
       </c>
       <c r="F3" t="s">
@@ -4411,7 +4402,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -4421,10 +4412,10 @@
       <c r="C4" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="83">
         <v>2</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="83">
         <v>8</v>
       </c>
       <c r="F4" t="s">
@@ -4437,62 +4428,62 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
       <c r="H5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>108</v>
       </c>
       <c r="B7" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>109</v>
       </c>
       <c r="B8" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-    </row>
-    <row r="11" spans="1:9" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+    </row>
+    <row r="11" spans="1:9" ht="70.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="35" t="s">
         <v>131</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="84" t="s">
         <v>139</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="84" t="s">
         <v>139</v>
       </c>
       <c r="F11" s="35" t="s">
@@ -4508,7 +4499,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -4523,7 +4514,7 @@
       <c r="H12" s="35"/>
       <c r="I12" s="35"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>144</v>
       </c>
@@ -4531,7 +4522,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -4548,7 +4539,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>135</v>
       </c>
@@ -4562,7 +4553,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>136</v>
       </c>
@@ -4576,7 +4567,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -4593,7 +4584,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>135</v>
       </c>
@@ -4607,7 +4598,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>136</v>
       </c>
@@ -4621,7 +4612,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>138</v>
       </c>
@@ -4638,7 +4629,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>136</v>
       </c>
@@ -4652,7 +4643,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>135</v>
       </c>
@@ -4666,7 +4657,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>136</v>
       </c>
@@ -4674,7 +4665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>135</v>
       </c>

</xml_diff>